<commit_message>
list of external ontologies
</commit_message>
<xml_diff>
--- a/CJK/list of external ontology.xlsx
+++ b/CJK/list of external ontology.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkchang/Github/CJK/CJK/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="20340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>OAE</t>
   </si>
@@ -109,16 +120,74 @@
   </si>
   <si>
     <t>Cell Line Ontology</t>
+  </si>
+  <si>
+    <t>Experimental Factor Ontology</t>
+  </si>
+  <si>
+    <t>Environment Ontology</t>
+  </si>
+  <si>
+    <t>Physico-Chemical Methods and Properties</t>
+  </si>
+  <si>
+    <t>Gene Ontology</t>
+  </si>
+  <si>
+    <t>Information Artifact Ontology</t>
+  </si>
+  <si>
+    <t>National Cancer Innstitute Thesaurus</t>
+  </si>
+  <si>
+    <t>NanoParticle Ontology</t>
+  </si>
+  <si>
+    <t>Ontology of Adverse Events</t>
+  </si>
+  <si>
+    <t>Ontology of Biological and Clinical Statistics</t>
+  </si>
+  <si>
+    <t>Ontology for Biomedical Investigation</t>
+  </si>
+  <si>
+    <t>Phenotype quality Ontology</t>
+  </si>
+  <si>
+    <t>Statistics Ontology</t>
+  </si>
+  <si>
+    <t>Unit of Measurement Ontology</t>
+  </si>
+  <si>
+    <t>Human Phenotype Ontology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,13 +210,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -457,15 +542,16 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection sqref="A1:B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="53.28515625" customWidth="1"/>
+    <col min="2" max="2" width="53.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -473,7 +559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -481,7 +567,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -489,7 +575,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -497,7 +583,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -505,7 +591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -513,7 +599,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -521,7 +607,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -529,74 +615,116 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -604,5 +732,6 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>